<commit_message>
add evidence info, from A1 to A20
</commit_message>
<xml_diff>
--- a/Adieanimart/evidence.xlsx
+++ b/Adieanimart/evidence.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Крипта\___2022 new Airdrop and others\GON testnet\18\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Крипта\___2022 new Airdrop and others\GON testnet\18\Adieanimart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="799"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="87">
   <si>
     <t>TeamName</t>
   </si>
@@ -76,45 +76,12 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
   </si>
   <si>
@@ -143,6 +110,201 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>C0DD00576F3ECF918D1C90E88574B44A5F55EB20E0C297ED40B20FD7BE4D5C41</t>
+  </si>
+  <si>
+    <t>cosmoszones</t>
+  </si>
+  <si>
+    <t>83C401EF007B2A61B2AB67B0BB4BB21EC7305EBB029ABD259F8B63D91F68E4AE</t>
+  </si>
+  <si>
+    <t>czone0001</t>
+  </si>
+  <si>
+    <t>CB1C3F73663BC0835C691323F65FBEAC6A3D7B52FE60CB192D93E73997E4422F</t>
+  </si>
+  <si>
+    <t>czone0002</t>
+  </si>
+  <si>
+    <t>B990E495F17FEAF6B3B4951620A90B6048FEE06C458525AA16AF813C69D6</t>
+  </si>
+  <si>
+    <t>stars1w7dxthechpr96rmw0a5zmumxj0re8hjrytr8aqsl6vtfz6j5v3lszcl2ly</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>10C9F9CC5C33CD0108A40D68643AD3977F944CAB42E1D73A47A0260121C32A66</t>
+  </si>
+  <si>
+    <t>ibc/B79219140E17C130BC2899D3C1D75BD3A5C967A92623AA27DA4EBA98705D0890</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>A85C861C9BAED1CBB7B9B8B32439C25308E23FF4625C875810776522E8ADB493</t>
+  </si>
+  <si>
+    <t>9A26EEA713B6AE7BAFA64303B01BB6D1470F3047915F8BAFF4DFBD9E4ABA0AC6</t>
+  </si>
+  <si>
+    <t>ibc/633FD8A0D59B069366E2B9CF345BB1E0F1672F3E03652757FCFA79780E5C9D3F</t>
+  </si>
+  <si>
+    <t>czone0003</t>
+  </si>
+  <si>
+    <t>ibc/9FEFBA9E6BED6CAEF8028C436F064C40B0BABC39F5699E00664D338B1EC8CD70</t>
+  </si>
+  <si>
+    <t>czone0004</t>
+  </si>
+  <si>
+    <t>ibc/EED63BD1E118D4802603DFCD414B72FF5F1069C85BCE1DA04422D56347AF9798</t>
+  </si>
+  <si>
+    <t>czone0005</t>
+  </si>
+  <si>
+    <t>ibc/ADDE9395B4A62ECEBEDEB2D11ED93F932A9A8FA8DE1572124F3FF9CC282139EC</t>
+  </si>
+  <si>
+    <t>czone0006</t>
+  </si>
+  <si>
+    <t>ibc/BCCD49430F5891755F7064E33AABD316F61CFC1A2B18CA13D3121EA1603CBA97</t>
+  </si>
+  <si>
+    <t>czone0007</t>
+  </si>
+  <si>
+    <t>ibc/7938D40AE4CBEECF9EF5A2797868CDAE656B85B47F7DA21D42B44D9C9DF4F53F</t>
+  </si>
+  <si>
+    <t>czone0008</t>
+  </si>
+  <si>
+    <t>8176B9C7D957DE72C0B202252092BC60BBA8484366901CB8E8E89FFC8F544BC4</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>9D357C6B8F91AA392A9C47204BAA188FB89C983ED4CCEF2EFF0C475029A98BBD</t>
+  </si>
+  <si>
+    <t>1679ABD8A91ED6AE1205F2A3D7506B38872B45C06A76527B86587A251A448AFD</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>5D26FA026D2E3C297ADFB8B539123B4C0C82F42C86035B4FB5D4496A989DF9BE</t>
+  </si>
+  <si>
+    <t>C4EDD962012061DE2D79E55B67E9E19EF253709979C7CAAA99DB915C4ACC9A8D</t>
+  </si>
+  <si>
+    <t>3E1073C0E808DD03B5D740DC04F30D39F51C339D5DB99DC7851C95AE71546BCE</t>
+  </si>
+  <si>
+    <t>7FF7AC970CB0F2E20E8A70DC972B0ABF33ED22327784875804CD5DD6441D52F6</t>
+  </si>
+  <si>
+    <t>F8B3A1B1FBC982EE1024B5A65D53D8A5CCB0A58BDBED81E27A1109E16AD45114</t>
+  </si>
+  <si>
+    <t>8D724E857158BB6D62A9C53F5CE409BCDCB70749992B422E79D0D02921412553</t>
+  </si>
+  <si>
+    <t>A2DF74ADE62B592B10FFC3641EB546D623514EDC4187C5D24560B1649B56330C</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>64785ED9C5ED3470C7E78271563B6A2C2553781396F75E87CAE8BC1F964CCB6B</t>
+  </si>
+  <si>
+    <t>387E4E865271B871C802088BDFD0B0407DD4B510E3515D808FB16011108D90EE</t>
+  </si>
+  <si>
+    <t>A0F492B51B5FA04C8002A8099A982350D217987ED763BC2448C6AE1BF8051320</t>
+  </si>
+  <si>
+    <t>E9113DD4F8DC9769E743F0DE19BB43BBF121A399CBF5FEF72A1912F7056533D7</t>
+  </si>
+  <si>
+    <t>9B4D821BBEE8FCD733D53724110DE5466936C94F9D7B4876F01E185A6590EECC</t>
+  </si>
+  <si>
+    <t>B3AB3614D15E8D5170F72A19601F01CE0FAAE1A6C89D0A1D6099E7CC92DFD4DA</t>
+  </si>
+  <si>
+    <t>DE4A469D583F389CF85D360A7AA82E86234DDE44B83D4A9FF7F79BF023E8B2E7</t>
+  </si>
+  <si>
+    <t>64BA91E1CE770C33715007947880D81E6E449FD68B9DA8D43EF9FCFC7FE5BC19</t>
+  </si>
+  <si>
+    <t>D0151552B9DAC0011A2AE99EC510DE34F9E9A6356EF8A68841F97350D05FA1BC</t>
+  </si>
+  <si>
+    <t>E93BB15CABE7F11610DE3905F45285B83E0E5D952E193EAAF1D363BE30F35F47</t>
+  </si>
+  <si>
+    <t>8DD2B5947A6AEDCA426BDFFE3BD6F30DE6BA3545A31BC6000E2ED55453D28F76</t>
+  </si>
+  <si>
+    <t>EAED7C5F8F4224DE76C8A7D9152E3EF79B212EEAB62ADB17EED9186752375218</t>
+  </si>
+  <si>
+    <t>7655DEB55B920EDD3B3FB2197CD9ECFAFA1D842E82D819989AA2C9EB4B857AC0</t>
+  </si>
+  <si>
+    <t>2FB602F2A4DDDF71C628987214D7E3BA6EB1E02807E08C6AFBC03149B202F08D</t>
+  </si>
+  <si>
+    <t>8E0C948FE47C39B9FB310F1212583435F3137DCCF8A4FA4121A247A3B06D3996</t>
+  </si>
+  <si>
+    <t>EB5C903A3C464E0F67EE5DB32EE885683E4F26D26BE3EFBB788A1DFC3D0DFD0C</t>
+  </si>
+  <si>
+    <t>A14FCC4EF88F0086CB3E68084C85FEDF6D28845FF3FF5B1CE579DF0EBF0434A7</t>
+  </si>
+  <si>
+    <t>EFFA1EAD2C70C5AA89FC253E15640B60DFFB0672B3C824366EDD6F03935152B3</t>
+  </si>
+  <si>
+    <t>A907C2A02DDC18E3FF163E6AC17B127514EF58BC65A32539310B861DD13C6C7A</t>
+  </si>
+  <si>
+    <t>7E6020D5E5978B1049242DF0209ADAC5A942DC3B1DFF9A5F97F54E125A7C8270</t>
+  </si>
+  <si>
+    <t>BABE58501A9DCC05AAF5CF82EC130229D3403C7C632613D9706F4483605EB25B</t>
+  </si>
+  <si>
+    <t>BB79EFDEFC165B1CC405406A331401471444D693A95B08C90F3455A6B25E3F3F</t>
+  </si>
+  <si>
+    <t>370417E2504309BEE158F3AEEC9F4B93B1B9CF3E618EC68BF322EE019E1B5B0F</t>
+  </si>
+  <si>
+    <t>51413F18B1E6502EE6FFDC3069BA9FB8353A5E50EAC249CF692C7A4BC6715BFE</t>
+  </si>
+  <si>
+    <t>78B55DECEAF5E7926A00C8F424D87F68DB105F544EE59471777BB2D487ACA473</t>
+  </si>
+  <si>
+    <t>C9E3EA440A2308E4B07B69E944FEDD478076451D2328D004FF71E29365256F78</t>
   </si>
 </sst>
 </file>
@@ -217,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -236,6 +398,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -582,7 +751,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,28 +794,28 @@
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -659,7 +828,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -672,15 +843,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -693,7 +864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -706,15 +879,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -740,15 +915,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +936,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -774,15 +951,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -793,14 +970,16 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -808,43 +987,470 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.88671875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
+      <c r="A3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -852,322 +1458,55 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
+      <c r="A2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
+      <c r="A3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="17.88671875" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
+      <c r="A4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1194,12 +1533,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1226,12 +1565,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1258,12 +1597,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1292,12 +1631,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1323,12 +1662,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1338,9 +1677,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1356,18 +1697,29 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
+      <c r="A2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1380,7 +1732,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1397,24 +1751,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1427,7 +1781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1444,24 +1800,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1474,7 +1830,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1491,24 +1849,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1521,7 +1879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1539,24 +1899,24 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1569,7 +1929,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1582,15 +1944,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1603,7 +1965,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1616,15 +1980,15 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>